<commit_message>
Fixes #3, #4, #5. Adds tests for #3, #5.
</commit_message>
<xml_diff>
--- a/data-raw/ols.xlsx
+++ b/data-raw/ols.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/Documents/GitHub/development/rorqual.morpho/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9233004B-CA99-064F-90CA-5F9F13319BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F362CA5-18E4-3F44-950A-27B5F9A52493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47720" yWindow="200" windowWidth="28040" windowHeight="17040" xr2:uid="{643C4424-97B3-3443-AC7E-1964ECF08AAE}"/>
+    <workbookView xWindow="18680" yWindow="460" windowWidth="10000" windowHeight="17540" xr2:uid="{643C4424-97B3-3443-AC7E-1964ECF08AAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -575,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3686299-D649-3842-A903-F0E1C45618BB}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,7 +590,7 @@
     <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -621,10 +621,10 @@
         <v>3.6671149999999999</v>
       </c>
       <c r="E2" s="5">
-        <v>-3.0245799999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>-1.4704366287839665E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -638,10 +638,10 @@
         <v>3.5488300000000002</v>
       </c>
       <c r="E3" s="5">
-        <v>-2.85446</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.15541563371216016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -655,10 +655,10 @@
         <v>3.2460300000000002</v>
       </c>
       <c r="E4" s="5">
-        <v>-2.1515</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.85837563371216019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -672,10 +672,10 @@
         <v>3.11151</v>
       </c>
       <c r="E5" s="5">
-        <v>-2.3132799999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.69659563371216038</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -689,10 +689,10 @@
         <v>3.1206</v>
       </c>
       <c r="E6" s="5">
-        <v>-2.4039000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.60597563371216001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -706,10 +706,10 @@
         <v>3.0556299999999998</v>
       </c>
       <c r="E7" s="5">
-        <v>-2.2380900000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.77178563371216002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
@@ -725,10 +725,10 @@
       <c r="E8" s="4">
         <v>-0.86146999999999996</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -744,10 +744,10 @@
       <c r="E9" s="4">
         <v>-0.98040000000000005</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -763,10 +763,10 @@
       <c r="E10" s="4">
         <v>-0.45795000000000002</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>8</v>
       </c>
@@ -782,10 +782,10 @@
       <c r="E11" s="4">
         <v>-1.0821000000000001</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
@@ -801,10 +801,10 @@
       <c r="E12" s="4">
         <v>-0.92290000000000005</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
@@ -820,10 +820,10 @@
       <c r="E13" s="4">
         <v>-0.93752999999999997</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>5</v>
       </c>
@@ -839,11 +839,10 @@
       <c r="E14" s="5">
         <v>-0.51300000000000001</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>6</v>
       </c>
@@ -859,11 +858,10 @@
       <c r="E15" s="5">
         <v>-0.76129000000000002</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>7</v>
       </c>
@@ -879,11 +877,10 @@
       <c r="E16" s="5">
         <v>-0.61699999999999999</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -899,11 +896,10 @@
       <c r="E17" s="5">
         <v>-0.64441999999999999</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
@@ -919,11 +915,10 @@
       <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>9</v>
       </c>
@@ -939,11 +934,10 @@
       <c r="E19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>5</v>
       </c>
@@ -959,9 +953,8 @@
       <c r="E20" s="4">
         <v>0.31290000000000001</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -978,7 +971,7 @@
         <v>1.2838799999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -995,7 +988,7 @@
         <v>1.8534999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1005,7 @@
         <v>2.1398999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>10</v>
       </c>
@@ -1029,7 +1022,7 @@
         <v>1.0765</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
@@ -1046,7 +1039,7 @@
         <v>1.4772000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>5</v>
       </c>
@@ -1062,10 +1055,9 @@
       <c r="E26" s="5">
         <v>-0.480657</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
@@ -1081,10 +1073,9 @@
       <c r="E27" s="5">
         <v>-0.45679999999999998</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
@@ -1100,10 +1091,9 @@
       <c r="E28" s="5">
         <v>-0.41249000000000002</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>8</v>
       </c>
@@ -1119,10 +1109,9 @@
       <c r="E29" s="5">
         <v>-0.51919000000000004</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>10</v>
       </c>
@@ -1138,10 +1127,9 @@
       <c r="E30" s="5">
         <v>-0.35980000000000001</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>9</v>
       </c>
@@ -1157,10 +1145,9 @@
       <c r="E31" s="5">
         <v>-0.18317</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
         <v>5</v>
       </c>
@@ -1176,10 +1163,9 @@
       <c r="E32" s="4">
         <v>-1.2198599999999999</v>
       </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
         <v>6</v>
       </c>
@@ -1195,10 +1181,9 @@
       <c r="E33" s="4">
         <v>-1.02603</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>7</v>
       </c>
@@ -1214,10 +1199,9 @@
       <c r="E34" s="4">
         <v>-0.83399000000000001</v>
       </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>8</v>
       </c>
@@ -1233,10 +1217,9 @@
       <c r="E35" s="4">
         <v>-0.69969000000000003</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>10</v>
       </c>
@@ -1252,10 +1235,9 @@
       <c r="E36" s="4">
         <v>-0.83472999999999997</v>
       </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>9</v>
       </c>
@@ -1271,10 +1253,9 @@
       <c r="E37" s="4">
         <v>-0.91046000000000005</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>5</v>
       </c>
@@ -1290,10 +1271,9 @@
       <c r="E38" s="5">
         <v>-1.1112500000000001</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>6</v>
       </c>
@@ -1309,10 +1289,9 @@
       <c r="E39" s="5">
         <v>-1.15882</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>7</v>
       </c>
@@ -1328,10 +1307,9 @@
       <c r="E40" s="5">
         <v>-0.69220999999999999</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>8</v>
       </c>
@@ -1347,10 +1325,9 @@
       <c r="E41" s="5">
         <v>-0.94350000000000001</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>10</v>
       </c>
@@ -1366,10 +1343,9 @@
       <c r="E42" s="5">
         <v>-1.0369999999999999</v>
       </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>9</v>
       </c>
@@ -1385,10 +1361,9 @@
       <c r="E43" s="5">
         <v>-0.93223</v>
       </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
         <v>5</v>
       </c>
@@ -1404,10 +1379,9 @@
       <c r="E44" s="4">
         <v>0.33271600000000001</v>
       </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
         <v>6</v>
       </c>
@@ -1423,10 +1397,9 @@
       <c r="E45" s="4">
         <v>0.95382999999999996</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
@@ -1442,10 +1415,9 @@
       <c r="E46" s="4">
         <v>0.90873000000000004</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>8</v>
       </c>
@@ -1461,10 +1433,9 @@
       <c r="E47" s="4">
         <v>1.2637</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
         <v>10</v>
       </c>
@@ -1480,10 +1451,9 @@
       <c r="E48" s="4">
         <v>3.1453000000000002</v>
       </c>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
         <v>9</v>
       </c>
@@ -1499,34 +1469,22 @@
       <c r="E49" s="4">
         <v>0.63210999999999995</v>
       </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G55" s="2"/>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G67" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>